<commit_message>
Using Page Object Model for efficiency
</commit_message>
<xml_diff>
--- a/Test_Data/Test_File.xlsx
+++ b/Test_Data/Test_File.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L&amp;T_Tech\Robot_Framework\Robot_Framework_Caption_Project\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04727CDD-9961-46C2-9C9C-A103FAC048DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723ADA6C-D394-4188-A529-BF600C84085E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{ED8F9148-88DF-4F8B-B0F7-AABB9F7EEF43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{ED8F9148-88DF-4F8B-B0F7-AABB9F7EEF43}"/>
   </bookViews>
   <sheets>
     <sheet name="Password_Validation" sheetId="1" r:id="rId1"/>
+    <sheet name="WishList_Addition" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>${username}</t>
   </si>
@@ -60,6 +61,45 @@
   </si>
   <si>
     <t>Please enter your password</t>
+  </si>
+  <si>
+    <t>${Items}</t>
+  </si>
+  <si>
+    <t>${Scroll}</t>
+  </si>
+  <si>
+    <t>cse20013@tezu.ac.in</t>
+  </si>
+  <si>
+    <t>usy253qu</t>
+  </si>
+  <si>
+    <t>xpath=//img[@alt='Duplex study table']</t>
+  </si>
+  <si>
+    <t>xpath=//img[@alt='Dash wall mounted study table']</t>
+  </si>
+  <si>
+    <t>xpath=//img[@alt='Tuck fold away work desk']</t>
+  </si>
+  <si>
+    <t>xpath=//img[@alt='POD 180 large study table']</t>
+  </si>
+  <si>
+    <t>xpath=//img[@alt='POD 180 small study table']</t>
+  </si>
+  <si>
+    <t>xpath=//img[@alt="Fluid portable study table"]</t>
+  </si>
+  <si>
+    <t>xpath=//img[@alt="Oblique study table"]</t>
+  </si>
+  <si>
+    <t>xpath=//img[@alt="Step-up compact study table"]</t>
+  </si>
+  <si>
+    <t>window.scrollTo(0,200)</t>
   </si>
 </sst>
 </file>
@@ -434,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C1D2B67-29EE-40BC-BCDB-8B6B2216D7CA}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -529,4 +569,210 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84AA4A72-196A-46D0-B691-181C8EEF8712}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{214EE06D-1CFA-4C4C-8237-B194481BF11B}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{74FBC888-77BF-4607-9883-C4E5E495AEF0}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{BF8FDBFF-17A8-4FCC-9C4E-4408A60E3563}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{DD9F91E0-99D2-439A-8759-7CCE11E00F0B}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{44EB3288-63B8-406D-8044-5110A01ACCFE}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{1AF83A23-2DFC-4EF1-B73C-FEE67BEAA174}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{BAF4C249-465F-47AA-8C6A-D6E90C9930D9}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{CF4A690E-E588-4169-87A0-5F3216309D77}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
+</worksheet>
 </file>
</xml_diff>